<commit_message>
filter RO at SOME wwtp
</commit_message>
<xml_diff>
--- a/inputs compound generator/inputs/excel_scenario.xlsx
+++ b/inputs compound generator/inputs/excel_scenario.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="447">
   <si>
     <t>codi_aca</t>
   </si>
@@ -1336,28 +1336,13 @@
     <t>SC</t>
   </si>
   <si>
-    <t>O3,SF,UV</t>
-  </si>
-  <si>
-    <t>UF,UV</t>
-  </si>
-  <si>
-    <t>SF,UV</t>
-  </si>
-  <si>
     <t>UF,CL</t>
   </si>
   <si>
     <t>UF,OTHER</t>
   </si>
   <si>
-    <t>O3,GAC,UV</t>
-  </si>
-  <si>
     <t>UF</t>
-  </si>
-  <si>
-    <t>GAC</t>
   </si>
   <si>
     <t>CL</t>
@@ -1775,9 +1760,6 @@
       <c r="F2" t="s">
         <v>437</v>
       </c>
-      <c r="G2" t="s">
-        <v>440</v>
-      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
@@ -2398,9 +2380,6 @@
       <c r="F33" t="s">
         <v>437</v>
       </c>
-      <c r="G33" t="s">
-        <v>441</v>
-      </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="1" t="s">
@@ -2421,9 +2400,6 @@
       <c r="F34" t="s">
         <v>437</v>
       </c>
-      <c r="G34" t="s">
-        <v>442</v>
-      </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="1" t="s">
@@ -2465,7 +2441,7 @@
         <v>439</v>
       </c>
       <c r="G36" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2507,9 +2483,6 @@
       <c r="F38" t="s">
         <v>438</v>
       </c>
-      <c r="G38" t="s">
-        <v>442</v>
-      </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="1" t="s">
@@ -2591,7 +2564,7 @@
         <v>438</v>
       </c>
       <c r="G42" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -2733,9 +2706,6 @@
       <c r="F49" t="s">
         <v>437</v>
       </c>
-      <c r="G49" t="s">
-        <v>445</v>
-      </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="1" t="s">
@@ -2757,7 +2727,7 @@
         <v>437</v>
       </c>
       <c r="G50" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -2899,9 +2869,6 @@
       <c r="F57" t="s">
         <v>437</v>
       </c>
-      <c r="G57" t="s">
-        <v>447</v>
-      </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="1" t="s">
@@ -3043,7 +3010,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:6">
       <c r="A65" s="1" t="s">
         <v>70</v>
       </c>
@@ -3063,7 +3030,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:6">
       <c r="A66" s="1" t="s">
         <v>71</v>
       </c>
@@ -3083,7 +3050,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:6">
       <c r="A67" s="1" t="s">
         <v>72</v>
       </c>
@@ -3103,7 +3070,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:6">
       <c r="A68" s="1" t="s">
         <v>73</v>
       </c>
@@ -3123,7 +3090,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:6">
       <c r="A69" s="1" t="s">
         <v>74</v>
       </c>
@@ -3143,7 +3110,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:6">
       <c r="A70" s="1" t="s">
         <v>75</v>
       </c>
@@ -3162,11 +3129,8 @@
       <c r="F70" t="s">
         <v>437</v>
       </c>
-      <c r="G70" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7">
+    </row>
+    <row r="71" spans="1:6">
       <c r="A71" s="1" t="s">
         <v>76</v>
       </c>
@@ -3186,7 +3150,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:6">
       <c r="A72" s="1" t="s">
         <v>77</v>
       </c>
@@ -3206,7 +3170,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:6">
       <c r="A73" s="1" t="s">
         <v>78</v>
       </c>
@@ -3226,7 +3190,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:6">
       <c r="A74" s="1" t="s">
         <v>79</v>
       </c>
@@ -3246,7 +3210,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:6">
       <c r="A75" s="1" t="s">
         <v>80</v>
       </c>
@@ -3266,7 +3230,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:6">
       <c r="A76" s="1" t="s">
         <v>81</v>
       </c>
@@ -3286,7 +3250,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:6">
       <c r="A77" s="1" t="s">
         <v>82</v>
       </c>
@@ -3306,7 +3270,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:6">
       <c r="A78" s="1" t="s">
         <v>83</v>
       </c>
@@ -3325,11 +3289,8 @@
       <c r="F78" t="s">
         <v>437</v>
       </c>
-      <c r="G78" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
+    </row>
+    <row r="79" spans="1:6">
       <c r="A79" s="1" t="s">
         <v>84</v>
       </c>
@@ -3349,7 +3310,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:6">
       <c r="A80" s="1" t="s">
         <v>85</v>
       </c>
@@ -3529,7 +3490,7 @@
         <v>437</v>
       </c>
       <c r="G88" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -3872,7 +3833,7 @@
         <v>438</v>
       </c>
       <c r="G105" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -4175,7 +4136,7 @@
         <v>437</v>
       </c>
       <c r="G120" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -4458,7 +4419,7 @@
         <v>439</v>
       </c>
       <c r="G134" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -4601,7 +4562,7 @@
         <v>437</v>
       </c>
       <c r="G141" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -4624,7 +4585,7 @@
         <v>437</v>
       </c>
       <c r="G142" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="143" spans="1:7">

</xml_diff>

<commit_message>
castellbell i vallbona afegits
</commit_message>
<xml_diff>
--- a/inputs compound generator/inputs/excel_scenario.xlsx
+++ b/inputs compound generator/inputs/excel_scenario.xlsx
@@ -499,7 +499,11 @@
           <t>SP</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>SF,UV</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -1460,7 +1464,11 @@
           <t>SP</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr"/>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>UF,UV</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
@@ -1491,7 +1499,11 @@
           <t>SP</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>O3,SF,UV</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
@@ -1619,7 +1631,11 @@
           <t>SN</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr"/>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>SF,UV</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
@@ -1964,7 +1980,11 @@
           <t>SP</t>
         </is>
       </c>
-      <c r="G49" t="inlineStr"/>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>GAC</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
@@ -2216,7 +2236,11 @@
           <t>SP</t>
         </is>
       </c>
-      <c r="G57" t="inlineStr"/>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>SF,UV</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
@@ -2619,7 +2643,11 @@
           <t>SP</t>
         </is>
       </c>
-      <c r="G70" t="inlineStr"/>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>UF,UV</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">

</xml_diff>

<commit_message>
lazy evaluation of scenarios
</commit_message>
<xml_diff>
--- a/inputs compound generator/inputs/excel_scenario.xlsx
+++ b/inputs compound generator/inputs/excel_scenario.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="452">
   <si>
     <t>codi_aca</t>
   </si>
@@ -1336,25 +1336,28 @@
     <t>SC</t>
   </si>
   <si>
+    <t>SF,UV</t>
+  </si>
+  <si>
+    <t>UF,UV</t>
+  </si>
+  <si>
+    <t>O3,SF,UV</t>
+  </si>
+  <si>
+    <t>UF,CL</t>
+  </si>
+  <si>
+    <t>UF,OTHER</t>
+  </si>
+  <si>
+    <t>UF</t>
+  </si>
+  <si>
+    <t>UF,RO,AOP</t>
+  </si>
+  <si>
     <t>O3,GAC,UV</t>
-  </si>
-  <si>
-    <t>SF,UV</t>
-  </si>
-  <si>
-    <t>UF,CL</t>
-  </si>
-  <si>
-    <t>UF,OTHER</t>
-  </si>
-  <si>
-    <t>UF</t>
-  </si>
-  <si>
-    <t>GAC</t>
-  </si>
-  <si>
-    <t>O3,SF</t>
   </si>
   <si>
     <t>CL</t>
@@ -2059,7 +2062,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -2079,7 +2082,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -2099,7 +2102,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -2118,8 +2121,11 @@
       <c r="F19" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -2139,7 +2145,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:7">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -2159,7 +2165,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:7">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -2179,7 +2185,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
@@ -2199,7 +2205,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
@@ -2219,7 +2225,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:7">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -2238,8 +2244,11 @@
       <c r="F25" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
@@ -2259,7 +2268,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:7">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
@@ -2279,7 +2288,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:7">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
@@ -2299,7 +2308,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:7">
       <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
@@ -2319,7 +2328,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:7">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
@@ -2339,7 +2348,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:7">
       <c r="A31" s="1" t="s">
         <v>36</v>
       </c>
@@ -2359,7 +2368,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:7">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
@@ -2398,6 +2407,9 @@
       <c r="F33" t="s">
         <v>437</v>
       </c>
+      <c r="G33" t="s">
+        <v>440</v>
+      </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="1" t="s">
@@ -2418,6 +2430,9 @@
       <c r="F34" t="s">
         <v>437</v>
       </c>
+      <c r="G34" t="s">
+        <v>440</v>
+      </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="1" t="s">
@@ -2459,7 +2474,7 @@
         <v>439</v>
       </c>
       <c r="G36" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2502,7 +2517,7 @@
         <v>438</v>
       </c>
       <c r="G38" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -2585,7 +2600,7 @@
         <v>438</v>
       </c>
       <c r="G42" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -2728,7 +2743,7 @@
         <v>437</v>
       </c>
       <c r="G49" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -2751,7 +2766,7 @@
         <v>437</v>
       </c>
       <c r="G50" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -2893,6 +2908,9 @@
       <c r="F57" t="s">
         <v>437</v>
       </c>
+      <c r="G57" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="1" t="s">
@@ -3154,7 +3172,7 @@
         <v>437</v>
       </c>
       <c r="G70" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -3317,7 +3335,7 @@
         <v>437</v>
       </c>
       <c r="G78" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -3520,7 +3538,7 @@
         <v>437</v>
       </c>
       <c r="G88" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -3863,7 +3881,7 @@
         <v>438</v>
       </c>
       <c r="G105" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -4166,7 +4184,7 @@
         <v>437</v>
       </c>
       <c r="G120" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -4449,7 +4467,7 @@
         <v>439</v>
       </c>
       <c r="G134" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -4592,7 +4610,7 @@
         <v>437</v>
       </c>
       <c r="G141" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -4615,7 +4633,7 @@
         <v>437</v>
       </c>
       <c r="G142" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="143" spans="1:7">

</xml_diff>